<commit_message>
'allocation version working fine'
</commit_message>
<xml_diff>
--- a/network_optimization/Inputs/Network_inputs_5airports.xlsx
+++ b/network_optimization/Inputs/Network_inputs_5airports.xlsx
@@ -5,38 +5,32 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarc8\Documents\Projects\network_optimization\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aarc8\Documents\GitHub\network_optimization\network_optimization\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D88B2C8-4155-40ED-8C56-BAE34DDB174C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7ADA98D-D7B9-43A0-B7C2-168E9703871B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Distances" sheetId="1" r:id="rId1"/>
     <sheet name="Demands" sheetId="2" r:id="rId2"/>
-    <sheet name="DOCs" sheetId="3" r:id="rId3"/>
-    <sheet name="Aircraft" sheetId="4" r:id="rId4"/>
+    <sheet name="Aircraft" sheetId="4" r:id="rId3"/>
+    <sheet name="DOC_1" sheetId="3" r:id="rId4"/>
+    <sheet name="DOC_2" sheetId="5" r:id="rId5"/>
+    <sheet name="DOC_3" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>acft_num</t>
   </si>
@@ -63,6 +57,12 @@
   </si>
   <si>
     <t>[8000,8000,5000,0]</t>
+  </si>
+  <si>
+    <t>[10000,10000,8000,0]</t>
+  </si>
+  <si>
+    <t>[12000,12000,9000,0]</t>
   </si>
 </sst>
 </file>
@@ -684,115 +684,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I20"/>
-  <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection sqref="A1:E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>6360</v>
-      </c>
-      <c r="C1">
-        <v>5029</v>
-      </c>
-      <c r="D1">
-        <v>4466</v>
-      </c>
-      <c r="E1">
-        <v>11562</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>6359</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>4324</v>
-      </c>
-      <c r="D2">
-        <v>4491</v>
-      </c>
-      <c r="E2">
-        <v>10372</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4985</v>
-      </c>
-      <c r="B3">
-        <v>4306</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>4662</v>
-      </c>
-      <c r="E3">
-        <v>9114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4468</v>
-      </c>
-      <c r="B4">
-        <v>4499</v>
-      </c>
-      <c r="C4">
-        <v>4668</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>11843</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>11470</v>
-      </c>
-      <c r="B5">
-        <v>10277</v>
-      </c>
-      <c r="C5">
-        <v>9038</v>
-      </c>
-      <c r="D5">
-        <v>11689</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I20" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDC8DBB-5558-40BE-A853-5A31B0E5D32D}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,7 +765,7 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
@@ -892,10 +788,317 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>6831</v>
+      </c>
+      <c r="C1">
+        <v>4849</v>
+      </c>
+      <c r="D1">
+        <v>4053</v>
+      </c>
+      <c r="E1">
+        <v>14477</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>6831</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>3878</v>
+      </c>
+      <c r="D2">
+        <v>4088</v>
+      </c>
+      <c r="E2">
+        <v>12653</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4849</v>
+      </c>
+      <c r="B3">
+        <v>3878</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>4351</v>
+      </c>
+      <c r="E3">
+        <v>10879</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4053</v>
+      </c>
+      <c r="B4">
+        <v>4088</v>
+      </c>
+      <c r="C4">
+        <v>4351</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>14859</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>14477</v>
+      </c>
+      <c r="B5">
+        <v>12653</v>
+      </c>
+      <c r="C5">
+        <v>10879</v>
+      </c>
+      <c r="D5">
+        <v>14859</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBCE523-71A3-44EE-88AC-D4A6E0363535}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="A1:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>6831</v>
+      </c>
+      <c r="C1">
+        <v>4849</v>
+      </c>
+      <c r="D1">
+        <v>4053</v>
+      </c>
+      <c r="E1">
+        <v>14477</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>6831</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>3878</v>
+      </c>
+      <c r="D2">
+        <v>4088</v>
+      </c>
+      <c r="E2">
+        <v>12653</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4849</v>
+      </c>
+      <c r="B3">
+        <v>3878</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>4351</v>
+      </c>
+      <c r="E3">
+        <v>10879</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4053</v>
+      </c>
+      <c r="B4">
+        <v>4088</v>
+      </c>
+      <c r="C4">
+        <v>4351</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>14859</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>14477</v>
+      </c>
+      <c r="B5">
+        <v>12653</v>
+      </c>
+      <c r="C5">
+        <v>10879</v>
+      </c>
+      <c r="D5">
+        <v>14859</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D19C95-93A5-4215-8C37-F781ABC52B12}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>5000</v>
+      </c>
+      <c r="C1">
+        <v>4849</v>
+      </c>
+      <c r="D1">
+        <v>4053</v>
+      </c>
+      <c r="E1">
+        <v>14477</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>6831</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>3878</v>
+      </c>
+      <c r="D2">
+        <v>4088</v>
+      </c>
+      <c r="E2">
+        <v>12653</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1254</v>
+      </c>
+      <c r="B3">
+        <v>4552</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>4351</v>
+      </c>
+      <c r="E3">
+        <v>10879</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4053</v>
+      </c>
+      <c r="B4">
+        <v>5222</v>
+      </c>
+      <c r="C4">
+        <v>4351</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>14859</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4000</v>
+      </c>
+      <c r="B5">
+        <v>12653</v>
+      </c>
+      <c r="C5">
+        <v>10879</v>
+      </c>
+      <c r="D5">
+        <v>14859</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>